<commit_message>
Assignment 1 Ready for upload
</commit_message>
<xml_diff>
--- a/Project Risks Table.xlsx
+++ b/Project Risks Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\University\Level 5- Software Development\Git Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{885557EA-8FBD-4FCC-9F04-0BFAAB5377DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AD6E2D-1567-4E5D-9C8F-1EC9F6CFAA97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{7716162D-6D61-49A4-8847-1490BA2A1EC9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t xml:space="preserve">Risk </t>
   </si>
@@ -63,18 +63,12 @@
     <t>We all need to research weather prediction algorithms and how they work/can be implemented </t>
   </si>
   <si>
-    <t>Missing a Project meeting </t>
-  </si>
-  <si>
     <t>If someone misses the meeting, they will not be up to date with progress, the next tasks and deadlines </t>
   </si>
   <si>
     <t>Minutes of each meeting will be recorded. All tasks will be updated on Jira with due dates, and assignees </t>
   </si>
   <si>
-    <t>Programming Issues </t>
-  </si>
-  <si>
     <t>Low </t>
   </si>
   <si>
@@ -82,6 +76,39 @@
   </si>
   <si>
     <t>Extensive testing throughout development </t>
+  </si>
+  <si>
+    <t>Increased time on tasks. Or increase workload for those with C# experience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carry out training so the whole team has a basic understanidng of the programming language </t>
+  </si>
+  <si>
+    <t>Missing a project meeting </t>
+  </si>
+  <si>
+    <t>Programming issues </t>
+  </si>
+  <si>
+    <t>Lack of C# experience</t>
+  </si>
+  <si>
+    <t>Conduct research on database building</t>
+  </si>
+  <si>
+    <t>An unsuitable database will be created that will store weather and user data incorrectly</t>
+  </si>
+  <si>
+    <t>Little experience in database building/ management</t>
+  </si>
+  <si>
+    <t>Little experience in server development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We may struggle to successfully store our database  </t>
+  </si>
+  <si>
+    <t>We will need to research how to sufficiently create a server that will support a database</t>
   </si>
 </sst>
 </file>
@@ -163,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -184,6 +211,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -500,19 +530,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE0CB92-E71E-437F-81D6-2EFAC2634093}">
-  <dimension ref="C2:J5"/>
+  <dimension ref="C2:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:I5"/>
+      <selection activeCell="C2" sqref="C2:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="8.140625" customWidth="1"/>
     <col min="5" max="5" width="10.140625" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -540,7 +570,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="3:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
@@ -560,57 +590,126 @@
         <v>9</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="3:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="H4" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="H5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="C6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="1"/>
+      <c r="H6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>